<commit_message>
formatting and new item-names.csv
</commit_message>
<xml_diff>
--- a/references/Release9_DataDic/ESWAN.xlsx
+++ b/references/Release9_DataDic/ESWAN.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/Research/Healthy Brain Network/Data Sharing/Data Dictionaries/Public Data Dictionaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Ksenia\Add Values\2files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="2120" windowWidth="25040" windowHeight="17820" tabRatio="500"/>
+    <workbookView xWindow="1884" yWindow="2124" windowWidth="25044" windowHeight="17820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="149">
   <si>
     <t>Question</t>
   </si>
@@ -508,7 +506,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -608,7 +606,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -616,7 +614,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -656,6 +653,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -986,32 +986,32 @@
   <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="89.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="89.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="21">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>147</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="6"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1021,33 +1021,33 @@
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="6" t="s">
         <v>130</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" ht="112" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="109.2">
+      <c r="A6" s="6" t="s">
         <v>131</v>
       </c>
       <c r="B6" t="s">
@@ -1056,18 +1056,18 @@
       <c r="C6" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="15" t="s">
+      <c r="D6" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>146</v>
       </c>
       <c r="F6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:6" ht="109.2">
+      <c r="A7" s="6" t="s">
         <v>132</v>
       </c>
       <c r="B7" t="s">
@@ -1076,13 +1076,15 @@
       <c r="C7" t="s">
         <v>145</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="D7" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="109.2">
+      <c r="A8" s="12" t="s">
         <v>133</v>
       </c>
       <c r="B8" t="s">
@@ -1091,12 +1093,15 @@
       <c r="C8" t="s">
         <v>145</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="D8" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="109.2">
+      <c r="A9" s="12" t="s">
         <v>134</v>
       </c>
       <c r="B9" t="s">
@@ -1105,12 +1110,15 @@
       <c r="C9" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="D9" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="109.2">
+      <c r="A10" s="11" t="s">
         <v>135</v>
       </c>
       <c r="B10" t="s">
@@ -1119,12 +1127,15 @@
       <c r="C10" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="D10" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="109.2">
+      <c r="A11" s="12" t="s">
         <v>136</v>
       </c>
       <c r="B11" t="s">
@@ -1133,12 +1144,15 @@
       <c r="C11" t="s">
         <v>145</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="D11" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="109.2">
+      <c r="A12" s="12" t="s">
         <v>137</v>
       </c>
       <c r="B12" t="s">
@@ -1147,12 +1161,15 @@
       <c r="C12" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="D12" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="109.2">
+      <c r="A13" s="12" t="s">
         <v>138</v>
       </c>
       <c r="B13" t="s">
@@ -1161,12 +1178,15 @@
       <c r="C13" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+      <c r="D13" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="109.2">
+      <c r="A14" s="12" t="s">
         <v>139</v>
       </c>
       <c r="B14" t="s">
@@ -1175,12 +1195,15 @@
       <c r="C14" t="s">
         <v>145</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+      <c r="D14" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="109.2">
+      <c r="A15" s="12" t="s">
         <v>140</v>
       </c>
       <c r="B15" t="s">
@@ -1189,12 +1212,15 @@
       <c r="C15" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="D15" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="109.2">
+      <c r="A16" s="12" t="s">
         <v>141</v>
       </c>
       <c r="B16" t="s">
@@ -1203,12 +1229,15 @@
       <c r="C16" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+      <c r="D16" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="109.2">
+      <c r="A17" s="12" t="s">
         <v>142</v>
       </c>
       <c r="B17" t="s">
@@ -1217,12 +1246,15 @@
       <c r="C17" t="s">
         <v>145</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
+      <c r="D17" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="109.2">
+      <c r="A18" s="12" t="s">
         <v>143</v>
       </c>
       <c r="B18" t="s">
@@ -1231,21 +1263,26 @@
       <c r="C18" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="D18" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="9" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="11" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5" ht="109.2">
       <c r="A21" t="s">
         <v>123</v>
       </c>
@@ -1255,11 +1292,14 @@
       <c r="C21" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="109.2">
       <c r="A22" t="s">
         <v>124</v>
       </c>
@@ -1269,11 +1309,14 @@
       <c r="C22" t="s">
         <v>145</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D22" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="109.2">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -1283,11 +1326,14 @@
       <c r="C23" t="s">
         <v>145</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D23" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="109.2">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -1297,11 +1343,14 @@
       <c r="C24" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D24" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="109.2">
       <c r="A25" t="s">
         <v>127</v>
       </c>
@@ -1311,11 +1360,14 @@
       <c r="C25" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="109.2">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -1325,29 +1377,36 @@
       <c r="C26" t="s">
         <v>145</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="109.2">
       <c r="A27" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="D27" s="5"/>
+      <c r="E27" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="109.2">
+      <c r="A28" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="5"/>
+      <c r="E28" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="109.2">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -1357,11 +1416,14 @@
       <c r="C29" t="s">
         <v>145</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="109.2">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -1371,11 +1433,14 @@
       <c r="C30" t="s">
         <v>145</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D30" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="109.2">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -1385,11 +1450,14 @@
       <c r="C31" t="s">
         <v>145</v>
       </c>
-      <c r="D31" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="109.2">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -1399,11 +1467,14 @@
       <c r="C32" t="s">
         <v>145</v>
       </c>
-      <c r="D32" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D32" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="109.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -1413,11 +1484,14 @@
       <c r="C33" t="s">
         <v>145</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="109.2">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -1427,11 +1501,14 @@
       <c r="C34" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D34" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="109.2">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -1441,11 +1518,14 @@
       <c r="C35" t="s">
         <v>145</v>
       </c>
-      <c r="D35" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="109.2">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -1455,11 +1535,14 @@
       <c r="C36" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="109.2">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -1469,11 +1552,14 @@
       <c r="C37" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="109.2">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -1483,11 +1569,14 @@
       <c r="C38" t="s">
         <v>145</v>
       </c>
-      <c r="D38" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D38" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="109.2">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -1497,11 +1586,14 @@
       <c r="C39" t="s">
         <v>145</v>
       </c>
-      <c r="D39" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="109.2">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -1511,11 +1603,14 @@
       <c r="C40" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D40" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="109.2">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -1525,11 +1620,14 @@
       <c r="C41" t="s">
         <v>145</v>
       </c>
-      <c r="D41" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D41" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="109.2">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -1539,11 +1637,14 @@
       <c r="C42" t="s">
         <v>145</v>
       </c>
-      <c r="D42" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D42" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="109.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -1553,11 +1654,14 @@
       <c r="C43" t="s">
         <v>145</v>
       </c>
-      <c r="D43" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="109.2">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -1567,11 +1671,14 @@
       <c r="C44" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="109.2">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -1581,11 +1688,14 @@
       <c r="C45" t="s">
         <v>145</v>
       </c>
-      <c r="D45" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D45" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="109.2">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -1595,11 +1705,14 @@
       <c r="C46" t="s">
         <v>145</v>
       </c>
-      <c r="D46" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D46" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="109.2">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -1609,11 +1722,14 @@
       <c r="C47" t="s">
         <v>145</v>
       </c>
-      <c r="D47" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D47" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="109.2">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -1623,11 +1739,14 @@
       <c r="C48" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D48" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="109.2">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -1637,11 +1756,14 @@
       <c r="C49" t="s">
         <v>145</v>
       </c>
-      <c r="D49" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D49" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="109.2">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -1651,11 +1773,14 @@
       <c r="C50" t="s">
         <v>145</v>
       </c>
-      <c r="D50" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="109.2">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -1665,11 +1790,14 @@
       <c r="C51" t="s">
         <v>145</v>
       </c>
-      <c r="D51" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="109.2">
       <c r="A52" t="s">
         <v>96</v>
       </c>
@@ -1679,11 +1807,14 @@
       <c r="C52" t="s">
         <v>145</v>
       </c>
-      <c r="D52" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D52" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="109.2">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -1693,11 +1824,14 @@
       <c r="C53" t="s">
         <v>145</v>
       </c>
-      <c r="D53" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D53" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="109.2">
       <c r="A54" t="s">
         <v>98</v>
       </c>
@@ -1707,11 +1841,14 @@
       <c r="C54" t="s">
         <v>145</v>
       </c>
-      <c r="D54" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D54" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="109.2">
       <c r="A55" t="s">
         <v>99</v>
       </c>
@@ -1721,12 +1858,15 @@
       <c r="C55" t="s">
         <v>145</v>
       </c>
-      <c r="D55" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
+      <c r="D55" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="109.2">
+      <c r="A56" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B56" t="s">
@@ -1735,12 +1875,15 @@
       <c r="C56" t="s">
         <v>145</v>
       </c>
-      <c r="D56" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
+      <c r="D56" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="109.2">
+      <c r="A57" s="7" t="s">
         <v>101</v>
       </c>
       <c r="B57" t="s">
@@ -1749,12 +1892,15 @@
       <c r="C57" t="s">
         <v>145</v>
       </c>
-      <c r="D57" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
+      <c r="D57" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="109.2">
+      <c r="A58" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B58" t="s">
@@ -1763,22 +1909,27 @@
       <c r="C58" t="s">
         <v>145</v>
       </c>
-      <c r="D58" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="9" t="s">
+      <c r="D58" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="9" customFormat="1">
+      <c r="A59" s="8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="11" t="s">
+      <c r="E59" s="14"/>
+    </row>
+    <row r="60" spans="1:5" s="9" customFormat="1">
+      <c r="A60" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="11" t="s">
+      <c r="E60" s="14"/>
+    </row>
+    <row r="61" spans="1:5" ht="109.2">
+      <c r="A61" s="10" t="s">
         <v>104</v>
       </c>
       <c r="B61" t="s">
@@ -1787,12 +1938,15 @@
       <c r="C61" t="s">
         <v>145</v>
       </c>
-      <c r="D61" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="11" t="s">
+      <c r="D61" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="109.2">
+      <c r="A62" s="10" t="s">
         <v>105</v>
       </c>
       <c r="B62" t="s">
@@ -1801,12 +1955,15 @@
       <c r="C62" t="s">
         <v>145</v>
       </c>
-      <c r="D62" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="11" t="s">
+      <c r="D62" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="109.2">
+      <c r="A63" s="10" t="s">
         <v>106</v>
       </c>
       <c r="B63" t="s">
@@ -1815,17 +1972,21 @@
       <c r="C63" t="s">
         <v>145</v>
       </c>
-      <c r="D63" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A64" s="11" t="s">
+      <c r="D63" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="31.2">
+      <c r="A64" s="10" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="11" t="s">
+      <c r="E64" s="14"/>
+    </row>
+    <row r="65" spans="1:5" ht="109.2">
+      <c r="A65" s="10" t="s">
         <v>108</v>
       </c>
       <c r="B65" t="s">
@@ -1834,12 +1995,15 @@
       <c r="C65" t="s">
         <v>145</v>
       </c>
-      <c r="D65" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="11" t="s">
+      <c r="D65" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="109.2">
+      <c r="A66" s="10" t="s">
         <v>109</v>
       </c>
       <c r="B66" t="s">
@@ -1848,12 +2012,15 @@
       <c r="C66" t="s">
         <v>145</v>
       </c>
-      <c r="D66" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="11" t="s">
+      <c r="D66" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="109.2">
+      <c r="A67" s="10" t="s">
         <v>110</v>
       </c>
       <c r="B67" t="s">
@@ -1862,12 +2029,15 @@
       <c r="C67" t="s">
         <v>145</v>
       </c>
-      <c r="D67" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="11" t="s">
+      <c r="D67" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="109.2">
+      <c r="A68" s="10" t="s">
         <v>111</v>
       </c>
       <c r="B68" t="s">
@@ -1876,12 +2046,15 @@
       <c r="C68" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="11" t="s">
+      <c r="D68" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="109.2">
+      <c r="A69" s="10" t="s">
         <v>112</v>
       </c>
       <c r="B69" t="s">
@@ -1890,12 +2063,15 @@
       <c r="C69" t="s">
         <v>145</v>
       </c>
-      <c r="D69" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="11" t="s">
+      <c r="D69" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="109.2">
+      <c r="A70" s="10" t="s">
         <v>113</v>
       </c>
       <c r="B70" t="s">
@@ -1904,12 +2080,15 @@
       <c r="C70" t="s">
         <v>145</v>
       </c>
-      <c r="D70" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="11" t="s">
+      <c r="D70" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="109.2">
+      <c r="A71" s="10" t="s">
         <v>114</v>
       </c>
       <c r="B71" t="s">
@@ -1918,12 +2097,15 @@
       <c r="C71" t="s">
         <v>145</v>
       </c>
-      <c r="D71" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="11" t="s">
+      <c r="D71" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="109.2">
+      <c r="A72" s="10" t="s">
         <v>115</v>
       </c>
       <c r="B72" t="s">
@@ -1932,12 +2114,15 @@
       <c r="C72" t="s">
         <v>145</v>
       </c>
-      <c r="D72" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="11" t="s">
+      <c r="D72" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="109.2">
+      <c r="A73" s="10" t="s">
         <v>116</v>
       </c>
       <c r="B73" t="s">
@@ -1946,12 +2131,15 @@
       <c r="C73" t="s">
         <v>145</v>
       </c>
-      <c r="D73" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="11" t="s">
+      <c r="D73" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="109.2">
+      <c r="A74" s="10" t="s">
         <v>117</v>
       </c>
       <c r="B74" t="s">
@@ -1960,12 +2148,15 @@
       <c r="C74" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="11" t="s">
+      <c r="D74" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="109.2">
+      <c r="A75" s="10" t="s">
         <v>118</v>
       </c>
       <c r="B75" t="s">
@@ -1974,12 +2165,15 @@
       <c r="C75" t="s">
         <v>145</v>
       </c>
-      <c r="D75" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="11" t="s">
+      <c r="D75" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="109.2">
+      <c r="A76" s="10" t="s">
         <v>119</v>
       </c>
       <c r="B76" t="s">
@@ -1988,12 +2182,15 @@
       <c r="C76" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="11" t="s">
+      <c r="D76" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="109.2">
+      <c r="A77" s="10" t="s">
         <v>120</v>
       </c>
       <c r="B77" t="s">
@@ -2002,12 +2199,27 @@
       <c r="C77" t="s">
         <v>145</v>
       </c>
-      <c r="D77" s="14" t="s">
-        <v>144</v>
+      <c r="D77" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E77" s="14" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new data dicts for inverse response options + rename make_HBN
</commit_message>
<xml_diff>
--- a/references/Release9_DataDic/ESWAN.xlsx
+++ b/references/Release9_DataDic/ESWAN.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Ksenia\Add Values\2files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/home/Repos/hbn/diagnosis_predictor/references/Release9_DataDic/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826E0435-1392-144F-B1E0-7E7AC4BABCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="2124" windowWidth="25044" windowHeight="17820" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="580" windowWidth="18580" windowHeight="17340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -487,26 +488,26 @@
     <t>Numeric</t>
   </si>
   <si>
+    <t>*In order to calculate the score for each assessment, calculate the average of the item values</t>
+  </si>
+  <si>
+    <t>*Applies to all questions</t>
+  </si>
+  <si>
     <t>-3= Far above average
 -2= Above average
 -1= Slightly above average
 0= Average
 1= Slightly below average
-2= Above average
-3= Far above average</t>
-  </si>
-  <si>
-    <t>*In order to calculate the score for each assessment, calculate the average of the item values</t>
-  </si>
-  <si>
-    <t>*Applies to all questions</t>
+2= Below average
+3= Far below average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -606,32 +607,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -982,36 +976,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="89.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="89.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="21">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>129</v>
       </c>
@@ -1037,17 +1031,16 @@
       <c r="D4" s="5"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>130</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="109.2">
-      <c r="A6" s="6" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>131</v>
       </c>
       <c r="B6" t="s">
@@ -1056,18 +1049,18 @@
       <c r="C6" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>146</v>
+      <c r="D6" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>148</v>
       </c>
       <c r="F6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="109.2">
-      <c r="A7" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>132</v>
       </c>
       <c r="B7" t="s">
@@ -1076,15 +1069,15 @@
       <c r="C7" t="s">
         <v>145</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="109.2">
-      <c r="A8" s="12" t="s">
+      <c r="D7" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>133</v>
       </c>
       <c r="B8" t="s">
@@ -1093,15 +1086,15 @@
       <c r="C8" t="s">
         <v>145</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="109.2">
-      <c r="A9" s="12" t="s">
+      <c r="D8" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>134</v>
       </c>
       <c r="B9" t="s">
@@ -1110,15 +1103,15 @@
       <c r="C9" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="109.2">
-      <c r="A10" s="11" t="s">
+      <c r="D9" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>135</v>
       </c>
       <c r="B10" t="s">
@@ -1127,15 +1120,15 @@
       <c r="C10" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="109.2">
-      <c r="A11" s="12" t="s">
+      <c r="D10" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>136</v>
       </c>
       <c r="B11" t="s">
@@ -1144,15 +1137,15 @@
       <c r="C11" t="s">
         <v>145</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="109.2">
-      <c r="A12" s="12" t="s">
+      <c r="D11" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>137</v>
       </c>
       <c r="B12" t="s">
@@ -1161,15 +1154,15 @@
       <c r="C12" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="109.2">
-      <c r="A13" s="12" t="s">
+      <c r="D12" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>138</v>
       </c>
       <c r="B13" t="s">
@@ -1178,15 +1171,15 @@
       <c r="C13" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="109.2">
-      <c r="A14" s="12" t="s">
+      <c r="D13" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>139</v>
       </c>
       <c r="B14" t="s">
@@ -1195,15 +1188,15 @@
       <c r="C14" t="s">
         <v>145</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="109.2">
-      <c r="A15" s="12" t="s">
+      <c r="D14" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>140</v>
       </c>
       <c r="B15" t="s">
@@ -1212,15 +1205,15 @@
       <c r="C15" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="109.2">
-      <c r="A16" s="12" t="s">
+      <c r="D15" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>141</v>
       </c>
       <c r="B16" t="s">
@@ -1229,15 +1222,15 @@
       <c r="C16" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="109.2">
-      <c r="A17" s="12" t="s">
+      <c r="D16" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>142</v>
       </c>
       <c r="B17" t="s">
@@ -1246,15 +1239,15 @@
       <c r="C17" t="s">
         <v>145</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="109.2">
-      <c r="A18" s="12" t="s">
+      <c r="D17" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>143</v>
       </c>
       <c r="B18" t="s">
@@ -1263,26 +1256,26 @@
       <c r="C18" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="9" t="s">
+      <c r="D18" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="11" t="s">
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>122</v>
       </c>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="1:5" ht="109.2">
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>123</v>
       </c>
@@ -1292,14 +1285,14 @@
       <c r="C21" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="109.2">
+      <c r="D21" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>124</v>
       </c>
@@ -1309,14 +1302,14 @@
       <c r="C22" t="s">
         <v>145</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="109.2">
+      <c r="D22" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -1326,14 +1319,14 @@
       <c r="C23" t="s">
         <v>145</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="109.2">
+      <c r="D23" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -1343,14 +1336,14 @@
       <c r="C24" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="109.2">
+      <c r="D24" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>127</v>
       </c>
@@ -1360,14 +1353,14 @@
       <c r="C25" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="109.2">
+      <c r="D25" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -1377,36 +1370,32 @@
       <c r="C26" t="s">
         <v>145</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="109.2">
+      <c r="D26" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="109.2">
-      <c r="A28" s="6" t="s">
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="109.2">
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -1416,14 +1405,14 @@
       <c r="C29" t="s">
         <v>145</v>
       </c>
-      <c r="D29" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="109.2">
+      <c r="D29" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -1433,14 +1422,14 @@
       <c r="C30" t="s">
         <v>145</v>
       </c>
-      <c r="D30" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="109.2">
+      <c r="D30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -1450,14 +1439,14 @@
       <c r="C31" t="s">
         <v>145</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="109.2">
+      <c r="D31" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -1467,14 +1456,14 @@
       <c r="C32" t="s">
         <v>145</v>
       </c>
-      <c r="D32" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="109.2">
+      <c r="D32" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -1484,14 +1473,14 @@
       <c r="C33" t="s">
         <v>145</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="109.2">
+      <c r="D33" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -1501,14 +1490,14 @@
       <c r="C34" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="109.2">
+      <c r="D34" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -1518,14 +1507,14 @@
       <c r="C35" t="s">
         <v>145</v>
       </c>
-      <c r="D35" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="109.2">
+      <c r="D35" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -1535,14 +1524,14 @@
       <c r="C36" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="109.2">
+      <c r="D36" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -1552,14 +1541,14 @@
       <c r="C37" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="109.2">
+      <c r="D37" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -1569,14 +1558,14 @@
       <c r="C38" t="s">
         <v>145</v>
       </c>
-      <c r="D38" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="109.2">
+      <c r="D38" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -1586,14 +1575,14 @@
       <c r="C39" t="s">
         <v>145</v>
       </c>
-      <c r="D39" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="109.2">
+      <c r="D39" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -1603,14 +1592,14 @@
       <c r="C40" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="109.2">
+      <c r="D40" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -1620,14 +1609,14 @@
       <c r="C41" t="s">
         <v>145</v>
       </c>
-      <c r="D41" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="109.2">
+      <c r="D41" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -1637,14 +1626,14 @@
       <c r="C42" t="s">
         <v>145</v>
       </c>
-      <c r="D42" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="109.2">
+      <c r="D42" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -1654,14 +1643,14 @@
       <c r="C43" t="s">
         <v>145</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="109.2">
+      <c r="D43" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -1671,14 +1660,14 @@
       <c r="C44" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="109.2">
+      <c r="D44" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -1688,14 +1677,14 @@
       <c r="C45" t="s">
         <v>145</v>
       </c>
-      <c r="D45" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="109.2">
+      <c r="D45" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -1705,14 +1694,14 @@
       <c r="C46" t="s">
         <v>145</v>
       </c>
-      <c r="D46" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="109.2">
+      <c r="D46" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -1722,14 +1711,14 @@
       <c r="C47" t="s">
         <v>145</v>
       </c>
-      <c r="D47" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="109.2">
+      <c r="D47" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -1739,14 +1728,14 @@
       <c r="C48" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="109.2">
+      <c r="D48" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -1756,14 +1745,14 @@
       <c r="C49" t="s">
         <v>145</v>
       </c>
-      <c r="D49" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="109.2">
+      <c r="D49" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -1773,14 +1762,14 @@
       <c r="C50" t="s">
         <v>145</v>
       </c>
-      <c r="D50" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="109.2">
+      <c r="D50" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -1790,14 +1779,14 @@
       <c r="C51" t="s">
         <v>145</v>
       </c>
-      <c r="D51" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="109.2">
+      <c r="D51" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>96</v>
       </c>
@@ -1807,14 +1796,14 @@
       <c r="C52" t="s">
         <v>145</v>
       </c>
-      <c r="D52" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="109.2">
+      <c r="D52" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -1824,14 +1813,14 @@
       <c r="C53" t="s">
         <v>145</v>
       </c>
-      <c r="D53" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="109.2">
+      <c r="D53" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>98</v>
       </c>
@@ -1841,14 +1830,14 @@
       <c r="C54" t="s">
         <v>145</v>
       </c>
-      <c r="D54" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E54" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="109.2">
+      <c r="D54" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>99</v>
       </c>
@@ -1858,15 +1847,15 @@
       <c r="C55" t="s">
         <v>145</v>
       </c>
-      <c r="D55" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="109.2">
-      <c r="A56" s="7" t="s">
+      <c r="D55" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
         <v>100</v>
       </c>
       <c r="B56" t="s">
@@ -1875,15 +1864,15 @@
       <c r="C56" t="s">
         <v>145</v>
       </c>
-      <c r="D56" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="109.2">
-      <c r="A57" s="7" t="s">
+      <c r="D56" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B57" t="s">
@@ -1892,15 +1881,15 @@
       <c r="C57" t="s">
         <v>145</v>
       </c>
-      <c r="D57" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E57" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="109.2">
-      <c r="A58" s="7" t="s">
+      <c r="D57" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
         <v>102</v>
       </c>
       <c r="B58" t="s">
@@ -1909,27 +1898,31 @@
       <c r="C58" t="s">
         <v>145</v>
       </c>
-      <c r="D58" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E58" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="9" customFormat="1">
-      <c r="A59" s="8" t="s">
+      <c r="D58" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E59" s="14"/>
-    </row>
-    <row r="60" spans="1:5" s="9" customFormat="1">
-      <c r="A60" s="10" t="s">
+      <c r="E59" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E60" s="14"/>
-    </row>
-    <row r="61" spans="1:5" ht="109.2">
-      <c r="A61" s="10" t="s">
+      <c r="E60" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
         <v>104</v>
       </c>
       <c r="B61" t="s">
@@ -1938,15 +1931,15 @@
       <c r="C61" t="s">
         <v>145</v>
       </c>
-      <c r="D61" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="109.2">
-      <c r="A62" s="10" t="s">
+      <c r="D61" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
         <v>105</v>
       </c>
       <c r="B62" t="s">
@@ -1955,15 +1948,15 @@
       <c r="C62" t="s">
         <v>145</v>
       </c>
-      <c r="D62" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="109.2">
-      <c r="A63" s="10" t="s">
+      <c r="D62" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B63" t="s">
@@ -1972,21 +1965,21 @@
       <c r="C63" t="s">
         <v>145</v>
       </c>
-      <c r="D63" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="31.2">
-      <c r="A64" s="10" t="s">
+      <c r="D63" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E64" s="14"/>
-    </row>
-    <row r="65" spans="1:5" ht="109.2">
-      <c r="A65" s="10" t="s">
+      <c r="E64" s="9"/>
+    </row>
+    <row r="65" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
         <v>108</v>
       </c>
       <c r="B65" t="s">
@@ -1995,15 +1988,15 @@
       <c r="C65" t="s">
         <v>145</v>
       </c>
-      <c r="D65" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="109.2">
-      <c r="A66" s="10" t="s">
+      <c r="D65" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B66" t="s">
@@ -2012,15 +2005,15 @@
       <c r="C66" t="s">
         <v>145</v>
       </c>
-      <c r="D66" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E66" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="109.2">
-      <c r="A67" s="10" t="s">
+      <c r="D66" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A67" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B67" t="s">
@@ -2029,15 +2022,15 @@
       <c r="C67" t="s">
         <v>145</v>
       </c>
-      <c r="D67" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E67" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="109.2">
-      <c r="A68" s="10" t="s">
+      <c r="D67" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B68" t="s">
@@ -2046,15 +2039,15 @@
       <c r="C68" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E68" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="109.2">
-      <c r="A69" s="10" t="s">
+      <c r="D68" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B69" t="s">
@@ -2063,15 +2056,15 @@
       <c r="C69" t="s">
         <v>145</v>
       </c>
-      <c r="D69" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E69" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="109.2">
-      <c r="A70" s="10" t="s">
+      <c r="D69" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
         <v>113</v>
       </c>
       <c r="B70" t="s">
@@ -2080,15 +2073,15 @@
       <c r="C70" t="s">
         <v>145</v>
       </c>
-      <c r="D70" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E70" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="109.2">
-      <c r="A71" s="10" t="s">
+      <c r="D70" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A71" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B71" t="s">
@@ -2097,15 +2090,15 @@
       <c r="C71" t="s">
         <v>145</v>
       </c>
-      <c r="D71" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E71" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="109.2">
-      <c r="A72" s="10" t="s">
+      <c r="D71" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A72" s="6" t="s">
         <v>115</v>
       </c>
       <c r="B72" t="s">
@@ -2114,15 +2107,15 @@
       <c r="C72" t="s">
         <v>145</v>
       </c>
-      <c r="D72" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E72" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="109.2">
-      <c r="A73" s="10" t="s">
+      <c r="D72" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A73" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B73" t="s">
@@ -2131,15 +2124,15 @@
       <c r="C73" t="s">
         <v>145</v>
       </c>
-      <c r="D73" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E73" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="109.2">
-      <c r="A74" s="10" t="s">
+      <c r="D73" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A74" s="6" t="s">
         <v>117</v>
       </c>
       <c r="B74" t="s">
@@ -2148,15 +2141,15 @@
       <c r="C74" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E74" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="109.2">
-      <c r="A75" s="10" t="s">
+      <c r="D74" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
         <v>118</v>
       </c>
       <c r="B75" t="s">
@@ -2165,15 +2158,15 @@
       <c r="C75" t="s">
         <v>145</v>
       </c>
-      <c r="D75" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E75" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="109.2">
-      <c r="A76" s="10" t="s">
+      <c r="D75" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A76" s="6" t="s">
         <v>119</v>
       </c>
       <c r="B76" t="s">
@@ -2182,15 +2175,15 @@
       <c r="C76" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E76" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="109.2">
-      <c r="A77" s="10" t="s">
+      <c r="D76" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A77" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B77" t="s">
@@ -2199,11 +2192,11 @@
       <c r="C77" t="s">
         <v>145</v>
       </c>
-      <c r="D77" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E77" s="14" t="s">
-        <v>146</v>
+      <c r="D77" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2213,12 +2206,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>